<commit_message>
Changes in design pattern selected and view one of the arquitecture.
</commit_message>
<xml_diff>
--- a/Evolucion Arquitectura.xlsx
+++ b/Evolucion Arquitectura.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Libranner\Dropbox\INTEC\INTEC AGO-OCT 2013\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-80" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="625" firstSheet="1" activeTab="3"/>
   </bookViews>
@@ -23,7 +18,7 @@
   <definedNames>
     <definedName name="_Toc366872465" localSheetId="1">'Utility tree'!$D$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="186">
   <si>
     <t>En horarios de máxima demanda, la creación de un reporte de avería para un recurso que requiere soporte externo, incluyendo la notificación al suplidor, debe completarse en 3 segundos.</t>
   </si>
@@ -137,7 +132,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
-        <family val="1"/>
       </rPr>
       <t>*, la creación de un reporte de avería para un recurso que requiere soporte externo, debe completarse en 2 segundos.</t>
     </r>
@@ -164,7 +158,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Cambria"/>
-        <family val="1"/>
       </rPr>
       <t>, el envio de notaficacion al suplidor debe hacerse en no mas de 1 segundo.</t>
     </r>
@@ -350,21 +343,12 @@
     <t>De los patrones candidatos se escogio MVC, puesto que la curva de aprendizaje era menor y cumple con las necesidades que presenta el proyecto.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hemos eliminado los "modelos" de la MVC de nuestro proyecto web y que lo incluya en la capa de lógica de negocios. También se elimina la capa de presentación periódica de la arquitectura de tres niveles y combinar eso con la parte delantera de la MVC. Esto significa que "Vistas" y "controladores" de la MVC representan la parte capa de presentación del sistema de tres niveles. </t>
-  </si>
-  <si>
-    <t>N-tier</t>
-  </si>
-  <si>
     <t>El patrón aísla "lógica de dominio" (la lógica de la aplicación para el usuario) de entrada y presentación (GUI), permitiendo desarrollos independientes, pruebas y mantenimiento de cada uno.</t>
   </si>
   <si>
     <t>VISTA 1</t>
   </si>
   <si>
-    <t>Capas es un patrón de diseño arquitectónico que las aplicaciones de estructuras por lo que se puede descomponer en grupos de subtareas de manera que cada grupo de subtareas está en un nivel particular de abstracción.Soporta la extensibilidad, modificabilidad, reusabilidad y bajo acoplamiento.</t>
-  </si>
-  <si>
     <t>Evaluar el diseño</t>
   </si>
   <si>
@@ -639,6 +623,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Responsive design</t>
+  </si>
+  <si>
+    <t>Patrón a utilizar</t>
   </si>
 </sst>
 </file>
@@ -802,7 +789,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +844,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -923,25 +916,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -958,11 +951,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -973,7 +966,7 @@
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1007,7 +1000,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1185,6 +1178,48 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="60"/>
     </xf>
@@ -1201,51 +1236,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1278,14 +1268,152 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1569,66 +1697,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1680,66 +1748,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1847,7 +1855,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-DO" sz="1100" baseline="0"/>
-            <a:t>BUSINESS LOGIC LAYER</a:t>
+            <a:t>Model</a:t>
           </a:r>
           <a:endParaRPr lang="es-DO" sz="1100"/>
         </a:p>
@@ -2224,10 +2232,9 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-DO" sz="1100" baseline="0"/>
-            <a:t>DATA ACCESS LAYER</a:t>
+            <a:rPr lang="es-DO" sz="1100"/>
+            <a:t>Database</a:t>
           </a:r>
-          <a:endParaRPr lang="es-DO" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3134,12 +3141,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B7:F20" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B7:F20" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
   <autoFilter ref="B7:F20"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Atributo de calidad"/>
     <tableColumn id="2" name="Attribute refinement"/>
-    <tableColumn id="3" name="ASR" dataDxfId="18"/>
+    <tableColumn id="3" name="ASR" dataDxfId="24"/>
     <tableColumn id="4" name="Business value"/>
     <tableColumn id="5" name="Arquitectural impact"/>
   </tableColumns>
@@ -3148,30 +3155,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="B7:G15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="B7:G15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22">
   <autoFilter ref="B7:G15"/>
   <sortState ref="B8:G15">
     <sortCondition ref="G7:G15"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Quality attribute" dataDxfId="8"/>
-    <tableColumn id="2" name="Attribute refinement" dataDxfId="7"/>
-    <tableColumn id="3" name="ASR" dataDxfId="6"/>
-    <tableColumn id="4" name="Business value" dataDxfId="5"/>
-    <tableColumn id="5" name="Arq. impact" dataDxfId="4"/>
-    <tableColumn id="6" name="#Iteracion" dataDxfId="3"/>
+    <tableColumn id="1" name="Quality attribute" dataDxfId="20"/>
+    <tableColumn id="2" name="Attribute refinement" dataDxfId="19"/>
+    <tableColumn id="3" name="ASR" dataDxfId="18"/>
+    <tableColumn id="4" name="Business value" dataDxfId="17"/>
+    <tableColumn id="5" name="Arq. impact" dataDxfId="16"/>
+    <tableColumn id="6" name="#Iteracion" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B18:B22" totalsRowShown="0" dataDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B18:B22" totalsRowShown="0" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="B18:B22">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Requerimientos funcionales 1era iteracion" dataDxfId="0"/>
+    <tableColumn id="1" name="Requerimientos funcionales 1era iteracion" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3501,11 +3508,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B45" sqref="B45:F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
@@ -3514,7 +3521,7 @@
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="18.5">
       <c r="E3" s="5">
         <v>1</v>
       </c>
@@ -3522,7 +3529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="18.5">
       <c r="E4" s="5">
         <v>2</v>
       </c>
@@ -3530,7 +3537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="18.5">
       <c r="B5" s="1"/>
       <c r="E5" s="5">
         <v>3</v>
@@ -3539,7 +3546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" ht="23.5">
       <c r="B6" s="59" t="s">
         <v>15</v>
       </c>
@@ -3548,7 +3555,7 @@
       <c r="E6" s="60"/>
       <c r="F6" s="61"/>
     </row>
-    <row r="7" spans="2:6" ht="21" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:6" ht="21">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -3565,57 +3572,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="45">
       <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="30">
       <c r="D9" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="45">
       <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="30">
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="60" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="60">
       <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="45" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="45">
       <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="90" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="90">
       <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="60" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="60">
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="75" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="75">
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="90" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="90">
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="30">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="7" t="s">
@@ -3624,7 +3631,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="30">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7" t="s">
@@ -3633,7 +3640,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="30">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7" t="s">
@@ -3642,7 +3649,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="45" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" ht="18.5">
       <c r="B45" s="62" t="s">
         <v>15</v>
       </c>
@@ -3651,7 +3658,7 @@
       <c r="E45" s="63"/>
       <c r="F45" s="64"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6">
       <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
@@ -3668,7 +3675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" ht="30">
       <c r="B47" s="23" t="s">
         <v>29</v>
       </c>
@@ -3685,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" ht="30">
       <c r="B48" s="23" t="s">
         <v>34</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" ht="31">
       <c r="B49" s="23" t="s">
         <v>32</v>
       </c>
@@ -3719,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" ht="31">
       <c r="B50" s="23" t="s">
         <v>41</v>
       </c>
@@ -3736,7 +3743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="45" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" ht="45">
       <c r="B51" s="23" t="s">
         <v>34</v>
       </c>
@@ -3753,7 +3760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" ht="30">
       <c r="B52" s="23" t="s">
         <v>34</v>
       </c>
@@ -3770,7 +3777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" ht="30">
       <c r="B53" s="23" t="s">
         <v>38</v>
       </c>
@@ -3787,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" ht="31">
       <c r="B54" s="23" t="s">
         <v>31</v>
       </c>
@@ -3804,7 +3811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" ht="31">
       <c r="B55" s="23" t="s">
         <v>38</v>
       </c>
@@ -3821,7 +3828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" ht="30">
       <c r="B56" s="23" t="s">
         <v>34</v>
       </c>
@@ -3838,7 +3845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" ht="31">
       <c r="B57" s="23" t="s">
         <v>38</v>
       </c>
@@ -3855,7 +3862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="30" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" ht="30">
       <c r="B58" s="23" t="s">
         <v>36</v>
       </c>
@@ -3878,24 +3885,24 @@
     <mergeCell ref="B45:F45"/>
   </mergeCells>
   <conditionalFormatting sqref="E47:E58">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:F58">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3920,17 +3927,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="37.4140625" customWidth="1"/>
-    <col min="3" max="3" width="35.4140625" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.25" style="37" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="42"/>
@@ -3941,7 +3948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7">
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
       <c r="D4" s="42"/>
@@ -3952,7 +3959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7">
       <c r="B5" s="42"/>
       <c r="C5" s="41"/>
       <c r="D5" s="42"/>
@@ -3963,9 +3970,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7">
       <c r="B6" s="65" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" s="65"/>
       <c r="D6" s="65"/>
@@ -3973,7 +3980,7 @@
       <c r="F6" s="65"/>
       <c r="G6" s="65"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7">
       <c r="B7" s="45" t="s">
         <v>46</v>
       </c>
@@ -3987,21 +3994,21 @@
         <v>12</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G7" s="48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="30">
       <c r="B8" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="12">
         <v>1</v>
@@ -4013,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="30">
       <c r="B9" s="12" t="s">
         <v>41</v>
       </c>
@@ -4021,7 +4028,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
@@ -4033,13 +4040,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="30">
       <c r="B10" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>
@@ -4051,15 +4058,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="45">
       <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E11" s="12">
         <v>1</v>
@@ -4071,15 +4078,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="30">
       <c r="B12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E12" s="12">
         <v>1</v>
@@ -4091,15 +4098,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="45">
       <c r="B13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E13" s="12">
         <v>1</v>
@@ -4111,7 +4118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="45">
       <c r="B14" s="12" t="s">
         <v>38</v>
       </c>
@@ -4119,7 +4126,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E14" s="12">
         <v>1</v>
@@ -4131,7 +4138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="30">
       <c r="B15" s="12" t="s">
         <v>38</v>
       </c>
@@ -4151,29 +4158,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="30">
+      <c r="B19" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="30" x14ac:dyDescent="0.35">
-      <c r="B19" s="12" t="s">
+    <row r="22" spans="2:2">
+      <c r="B22" s="58" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="58" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4181,33 +4188,38 @@
     <mergeCell ref="B6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F15">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E15">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4219,45 +4231,45 @@
       <selection activeCell="B2" sqref="B2:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="52.1640625" customWidth="1"/>
     <col min="3" max="3" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3">
       <c r="B2" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3">
       <c r="B3" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3">
       <c r="B4" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3">
       <c r="B5" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" ht="39.75" customHeight="1">
       <c r="B7" s="67" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="67"/>
     </row>
-    <row r="8" spans="2:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:3" ht="18.5">
       <c r="B8" s="66" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="66"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3">
       <c r="B9" s="14" t="s">
         <v>63</v>
       </c>
@@ -4265,7 +4277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" ht="31">
       <c r="B10" s="18" t="s">
         <v>65</v>
       </c>
@@ -4273,7 +4285,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" ht="31">
       <c r="B11" s="18" t="s">
         <v>67</v>
       </c>
@@ -4281,7 +4293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="31">
       <c r="B12" s="18" t="s">
         <v>68</v>
       </c>
@@ -4289,7 +4301,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" ht="31">
       <c r="B13" s="18" t="s">
         <v>69</v>
       </c>
@@ -4297,7 +4309,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" ht="31">
       <c r="B14" s="18" t="s">
         <v>70</v>
       </c>
@@ -4305,13 +4317,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" ht="31">
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" ht="46.5">
       <c r="B16" s="18" t="s">
         <v>75</v>
       </c>
@@ -4319,7 +4331,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3">
       <c r="B17" s="18" t="s">
         <v>77</v>
       </c>
@@ -4327,7 +4339,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="31">
       <c r="B18" s="18" t="s">
         <v>79</v>
       </c>
@@ -4335,7 +4347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="46.5">
       <c r="B19" s="18" t="s">
         <v>81</v>
       </c>
@@ -4343,7 +4355,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3">
       <c r="B20" s="18" t="s">
         <v>83</v>
       </c>
@@ -4351,7 +4363,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="37.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" ht="37.75" customHeight="1">
       <c r="B21" s="68" t="s">
         <v>90</v>
       </c>
@@ -4364,6 +4376,11 @@
     <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4371,37 +4388,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.5">
-      <c r="B3" s="79" t="s">
+    <row r="3" spans="2:10" ht="21">
+      <c r="B3" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-    </row>
-    <row r="4" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+    </row>
+    <row r="4" spans="2:10" ht="18.5">
       <c r="B4" s="66" t="s">
         <v>60</v>
       </c>
@@ -4416,71 +4433,71 @@
       </c>
       <c r="J4" s="80"/>
     </row>
-    <row r="5" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="76" t="s">
+    <row r="5" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1">
+      <c r="B5" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="81">
+        <v>1</v>
+      </c>
+      <c r="J5" s="82"/>
+    </row>
+    <row r="6" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1">
+      <c r="B6" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="81">
+        <v>2</v>
+      </c>
+      <c r="J6" s="82"/>
+    </row>
+    <row r="7" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1">
+      <c r="B7" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="74">
-        <v>1</v>
-      </c>
-      <c r="J5" s="75"/>
-    </row>
-    <row r="6" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="74">
-        <v>2</v>
-      </c>
-      <c r="J6" s="75"/>
-    </row>
-    <row r="7" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="76" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="74">
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="81">
         <v>3</v>
       </c>
-      <c r="J7" s="75"/>
-    </row>
-    <row r="8" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="74">
+      <c r="J7" s="82"/>
+    </row>
+    <row r="8" spans="2:10" s="20" customFormat="1" ht="15.5" customHeight="1">
+      <c r="B8" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="81">
         <v>4</v>
       </c>
-      <c r="J8" s="75"/>
-    </row>
-    <row r="9" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B9" s="70" t="s">
+      <c r="J8" s="82"/>
+    </row>
+    <row r="9" spans="2:10" ht="18.5">
+      <c r="B9" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="71"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="62" t="s">
         <v>59</v>
       </c>
@@ -4491,9 +4508,9 @@
       <c r="I9" s="63"/>
       <c r="J9" s="64"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
+    <row r="10" spans="2:10">
+      <c r="B10" s="86"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="19" t="s">
         <v>29</v>
       </c>
@@ -4514,18 +4531,18 @@
       </c>
       <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="69" t="s">
+    <row r="11" spans="2:10">
+      <c r="B11" s="83" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="21"/>
@@ -4533,33 +4550,33 @@
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="69"/>
+    <row r="12" spans="2:10">
+      <c r="B12" s="83"/>
       <c r="C12" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J12" s="21"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="69"/>
+    <row r="13" spans="2:10">
+      <c r="B13" s="83"/>
       <c r="C13" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
@@ -4567,8 +4584,8 @@
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="69"/>
+    <row r="14" spans="2:10">
+      <c r="B14" s="83"/>
       <c r="C14" s="11" t="s">
         <v>55</v>
       </c>
@@ -4580,10 +4597,10 @@
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="69"/>
+    <row r="15" spans="2:10">
+      <c r="B15" s="83"/>
       <c r="C15" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -4593,8 +4610,8 @@
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="69"/>
+    <row r="16" spans="2:10">
+      <c r="B16" s="83"/>
       <c r="C16" s="11" t="s">
         <v>56</v>
       </c>
@@ -4606,8 +4623,8 @@
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
     </row>
-    <row r="17" spans="2:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="B17" s="69"/>
+    <row r="17" spans="2:10" ht="31">
+      <c r="B17" s="83"/>
       <c r="C17" s="16" t="s">
         <v>57</v>
       </c>
@@ -4617,141 +4634,133 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="30" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J17" s="21"/>
     </row>
-    <row r="21" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:10" ht="15.5" customHeight="1">
       <c r="B21" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-    </row>
-    <row r="22" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.5" customHeight="1">
       <c r="B22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.5" customHeight="1">
+      <c r="B23" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.5" customHeight="1">
+      <c r="B24" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.5" customHeight="1">
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+    </row>
+    <row r="26" spans="2:10" ht="53.5" customHeight="1">
+      <c r="B26" s="99"/>
+      <c r="C26" s="99"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+    </row>
+    <row r="27" spans="2:10" ht="18.5" customHeight="1">
+      <c r="B27" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-    </row>
-    <row r="26" spans="2:10" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="67" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="67"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-    </row>
-    <row r="27" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="66"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-    </row>
-    <row r="28" spans="2:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="14" t="s">
+      <c r="C27" s="64"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+    </row>
+    <row r="28" spans="2:10" ht="15.5" customHeight="1">
+      <c r="B28" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-    </row>
-    <row r="29" spans="2:10" ht="124.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="18" t="s">
+      <c r="C28" s="102"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+    </row>
+    <row r="29" spans="2:10" ht="124.75" customHeight="1">
+      <c r="B29" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+    </row>
+    <row r="30" spans="2:10" ht="83.5" customHeight="1">
+      <c r="B30" s="104"/>
+      <c r="C30" s="104"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+    </row>
+    <row r="33" spans="2:10" ht="18.5">
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="E33" s="66" t="s">
         <v>93</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-    </row>
-    <row r="30" spans="2:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="68"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="84"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B32" s="86"/>
-      <c r="C32" s="86"/>
-    </row>
-    <row r="33" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="E33" s="66" t="s">
-        <v>96</v>
       </c>
       <c r="F33" s="66"/>
       <c r="G33" s="66"/>
@@ -4759,79 +4768,79 @@
       <c r="I33" s="66"/>
       <c r="J33" s="66"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B34" s="86"/>
-      <c r="C34" s="86"/>
-      <c r="E34" s="81" t="s">
+    <row r="34" spans="2:10">
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="E34" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="E35" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="24" t="s">
+    </row>
+    <row r="36" spans="2:10">
+      <c r="E36" s="71" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B35" s="86"/>
-      <c r="C35" s="86"/>
-      <c r="E35" s="82" t="s">
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="E37" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-      <c r="J35" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E36" s="82" t="s">
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="E38" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E37" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E38" s="82" t="s">
-        <v>104</v>
-      </c>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
       <c r="J38" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
       <c r="J39" s="25"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:10">
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -4839,7 +4848,7 @@
       <c r="I40" s="26"/>
       <c r="J40" s="27"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:10">
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
@@ -4847,9 +4856,9 @@
       <c r="I41" s="26"/>
       <c r="J41" s="27"/>
     </row>
-    <row r="44" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" ht="18.5">
       <c r="B44" s="66" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C44" s="66"/>
       <c r="D44" s="66"/>
@@ -4860,366 +4869,374 @@
       <c r="I44" s="66"/>
       <c r="J44" s="66"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B45" s="87"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-      <c r="F45" s="87"/>
-      <c r="G45" s="87"/>
-      <c r="H45" s="87"/>
-      <c r="I45" s="87"/>
-      <c r="J45" s="87"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B46" s="88"/>
-      <c r="C46" s="88"/>
-      <c r="D46" s="88"/>
-      <c r="E46" s="88"/>
-      <c r="F46" s="88"/>
-      <c r="G46" s="88"/>
-      <c r="H46" s="88"/>
-      <c r="I46" s="88"/>
-      <c r="J46" s="88"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B47" s="88"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="88"/>
-      <c r="F47" s="88"/>
-      <c r="G47" s="88"/>
-      <c r="H47" s="88"/>
-      <c r="I47" s="88"/>
-      <c r="J47" s="88"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B48" s="88"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="88"/>
-      <c r="I48" s="88"/>
-      <c r="J48" s="88"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B49" s="88"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
-      <c r="E49" s="88"/>
-      <c r="F49" s="88"/>
-      <c r="G49" s="88"/>
-      <c r="H49" s="88"/>
-      <c r="I49" s="88"/>
-      <c r="J49" s="88"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B50" s="88"/>
-      <c r="C50" s="88"/>
-      <c r="D50" s="88"/>
-      <c r="E50" s="88"/>
-      <c r="F50" s="88"/>
-      <c r="G50" s="88"/>
-      <c r="H50" s="88"/>
-      <c r="I50" s="88"/>
-      <c r="J50" s="88"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B51" s="88"/>
-      <c r="C51" s="88"/>
-      <c r="D51" s="88"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="88"/>
-      <c r="G51" s="88"/>
-      <c r="H51" s="88"/>
-      <c r="I51" s="88"/>
-      <c r="J51" s="88"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B52" s="88"/>
-      <c r="C52" s="88"/>
-      <c r="D52" s="88"/>
-      <c r="E52" s="88"/>
-      <c r="F52" s="88"/>
-      <c r="G52" s="88"/>
-      <c r="H52" s="88"/>
-      <c r="I52" s="88"/>
-      <c r="J52" s="88"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B53" s="88"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="88"/>
-      <c r="E53" s="88"/>
-      <c r="F53" s="88"/>
-      <c r="G53" s="88"/>
-      <c r="H53" s="88"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="88"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B54" s="88"/>
-      <c r="C54" s="88"/>
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="88"/>
-      <c r="I54" s="88"/>
-      <c r="J54" s="88"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B55" s="88"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="88"/>
-      <c r="G55" s="88"/>
-      <c r="H55" s="88"/>
-      <c r="I55" s="88"/>
-      <c r="J55" s="88"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B56" s="88"/>
-      <c r="C56" s="88"/>
-      <c r="D56" s="88"/>
-      <c r="E56" s="88"/>
-      <c r="F56" s="88"/>
-      <c r="G56" s="88"/>
-      <c r="H56" s="88"/>
-      <c r="I56" s="88"/>
-      <c r="J56" s="88"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B57" s="88"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="88"/>
-      <c r="H57" s="88"/>
-      <c r="I57" s="88"/>
-      <c r="J57" s="88"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="88"/>
-      <c r="H58" s="88"/>
-      <c r="I58" s="88"/>
-      <c r="J58" s="88"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="88"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="88"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="88"/>
-      <c r="G60" s="88"/>
-      <c r="H60" s="88"/>
-      <c r="I60" s="88"/>
-      <c r="J60" s="88"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B61" s="88"/>
-      <c r="C61" s="88"/>
-      <c r="D61" s="88"/>
-      <c r="E61" s="88"/>
-      <c r="F61" s="88"/>
-      <c r="G61" s="88"/>
-      <c r="H61" s="88"/>
-      <c r="I61" s="88"/>
-      <c r="J61" s="88"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B62" s="88"/>
-      <c r="C62" s="88"/>
-      <c r="D62" s="88"/>
-      <c r="E62" s="88"/>
-      <c r="F62" s="88"/>
-      <c r="G62" s="88"/>
-      <c r="H62" s="88"/>
-      <c r="I62" s="88"/>
-      <c r="J62" s="88"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B63" s="88"/>
-      <c r="C63" s="88"/>
-      <c r="D63" s="88"/>
-      <c r="E63" s="88"/>
-      <c r="F63" s="88"/>
-      <c r="G63" s="88"/>
-      <c r="H63" s="88"/>
-      <c r="I63" s="88"/>
-      <c r="J63" s="88"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B64" s="88"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="88"/>
-      <c r="E64" s="88"/>
-      <c r="F64" s="88"/>
-      <c r="G64" s="88"/>
-      <c r="H64" s="88"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="88"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B65" s="88"/>
-      <c r="C65" s="88"/>
-      <c r="D65" s="88"/>
-      <c r="E65" s="88"/>
-      <c r="F65" s="88"/>
-      <c r="G65" s="88"/>
-      <c r="H65" s="88"/>
-      <c r="I65" s="88"/>
-      <c r="J65" s="88"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B66" s="88"/>
-      <c r="C66" s="88"/>
-      <c r="D66" s="88"/>
-      <c r="E66" s="88"/>
-      <c r="F66" s="88"/>
-      <c r="G66" s="88"/>
-      <c r="H66" s="88"/>
-      <c r="I66" s="88"/>
-      <c r="J66" s="88"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B67" s="88"/>
-      <c r="C67" s="88"/>
-      <c r="D67" s="88"/>
-      <c r="E67" s="88"/>
-      <c r="F67" s="88"/>
-      <c r="G67" s="88"/>
-      <c r="H67" s="88"/>
-      <c r="I67" s="88"/>
-      <c r="J67" s="88"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B68" s="88"/>
-      <c r="C68" s="88"/>
-      <c r="D68" s="88"/>
-      <c r="E68" s="88"/>
-      <c r="F68" s="88"/>
-      <c r="G68" s="88"/>
-      <c r="H68" s="88"/>
-      <c r="I68" s="88"/>
-      <c r="J68" s="88"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B69" s="88"/>
-      <c r="C69" s="88"/>
-      <c r="D69" s="88"/>
-      <c r="E69" s="88"/>
-      <c r="F69" s="88"/>
-      <c r="G69" s="88"/>
-      <c r="H69" s="88"/>
-      <c r="I69" s="88"/>
-      <c r="J69" s="88"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B70" s="88"/>
-      <c r="C70" s="88"/>
-      <c r="D70" s="88"/>
-      <c r="E70" s="88"/>
-      <c r="F70" s="88"/>
-      <c r="G70" s="88"/>
-      <c r="H70" s="88"/>
-      <c r="I70" s="88"/>
-      <c r="J70" s="88"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B71" s="88"/>
-      <c r="C71" s="88"/>
-      <c r="D71" s="88"/>
-      <c r="E71" s="88"/>
-      <c r="F71" s="88"/>
-      <c r="G71" s="88"/>
-      <c r="H71" s="88"/>
-      <c r="I71" s="88"/>
-      <c r="J71" s="88"/>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B72" s="88"/>
-      <c r="C72" s="88"/>
-      <c r="D72" s="88"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="88"/>
-      <c r="G72" s="88"/>
-      <c r="H72" s="88"/>
-      <c r="I72" s="88"/>
-      <c r="J72" s="88"/>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B73" s="88"/>
-      <c r="C73" s="88"/>
-      <c r="D73" s="88"/>
-      <c r="E73" s="88"/>
-      <c r="F73" s="88"/>
-      <c r="G73" s="88"/>
-      <c r="H73" s="88"/>
-      <c r="I73" s="88"/>
-      <c r="J73" s="88"/>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B74" s="88"/>
-      <c r="C74" s="88"/>
-      <c r="D74" s="88"/>
-      <c r="E74" s="88"/>
-      <c r="F74" s="88"/>
-      <c r="G74" s="88"/>
-      <c r="H74" s="88"/>
-      <c r="I74" s="88"/>
-      <c r="J74" s="88"/>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B75" s="88"/>
-      <c r="C75" s="88"/>
-      <c r="D75" s="88"/>
-      <c r="E75" s="88"/>
-      <c r="F75" s="88"/>
-      <c r="G75" s="88"/>
-      <c r="H75" s="88"/>
-      <c r="I75" s="88"/>
-      <c r="J75" s="88"/>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B76" s="88"/>
-      <c r="C76" s="88"/>
-      <c r="D76" s="88"/>
-      <c r="E76" s="88"/>
-      <c r="F76" s="88"/>
-      <c r="G76" s="88"/>
-      <c r="H76" s="88"/>
-      <c r="I76" s="88"/>
-      <c r="J76" s="88"/>
+    <row r="45" spans="2:10">
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="70"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="70"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="70"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="70"/>
+      <c r="J47" s="70"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="70"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="70"/>
+      <c r="H48" s="70"/>
+      <c r="I48" s="70"/>
+      <c r="J48" s="70"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="70"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="70"/>
+      <c r="G49" s="70"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="70"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="70"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="70"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="70"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="70"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="70"/>
+      <c r="C53" s="70"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
+      <c r="J53" s="70"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="70"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
+      <c r="J54" s="70"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="70"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="70"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="70"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="70"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="70"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="70"/>
+      <c r="G56" s="70"/>
+      <c r="H56" s="70"/>
+      <c r="I56" s="70"/>
+      <c r="J56" s="70"/>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="70"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="70"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="70"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="70"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="70"/>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" s="70"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="70"/>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="70"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" s="70"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="70"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="70"/>
+      <c r="G61" s="70"/>
+      <c r="H61" s="70"/>
+      <c r="I61" s="70"/>
+      <c r="J61" s="70"/>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="70"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="70"/>
+      <c r="E62" s="70"/>
+      <c r="F62" s="70"/>
+      <c r="G62" s="70"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="70"/>
+      <c r="J62" s="70"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="70"/>
+      <c r="C63" s="70"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="70"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="70"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="70"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="70"/>
+      <c r="C65" s="70"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="70"/>
+      <c r="F65" s="70"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="70"/>
+      <c r="J65" s="70"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="70"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="70"/>
+      <c r="G66" s="70"/>
+      <c r="H66" s="70"/>
+      <c r="I66" s="70"/>
+      <c r="J66" s="70"/>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="70"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="70"/>
+      <c r="F67" s="70"/>
+      <c r="G67" s="70"/>
+      <c r="H67" s="70"/>
+      <c r="I67" s="70"/>
+      <c r="J67" s="70"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="70"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="70"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="70"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="70"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="70"/>
+      <c r="F69" s="70"/>
+      <c r="G69" s="70"/>
+      <c r="H69" s="70"/>
+      <c r="I69" s="70"/>
+      <c r="J69" s="70"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="B70" s="70"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="70"/>
+      <c r="E70" s="70"/>
+      <c r="F70" s="70"/>
+      <c r="G70" s="70"/>
+      <c r="H70" s="70"/>
+      <c r="I70" s="70"/>
+      <c r="J70" s="70"/>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="B71" s="70"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="70"/>
+      <c r="E71" s="70"/>
+      <c r="F71" s="70"/>
+      <c r="G71" s="70"/>
+      <c r="H71" s="70"/>
+      <c r="I71" s="70"/>
+      <c r="J71" s="70"/>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="70"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="70"/>
+      <c r="E72" s="70"/>
+      <c r="F72" s="70"/>
+      <c r="G72" s="70"/>
+      <c r="H72" s="70"/>
+      <c r="I72" s="70"/>
+      <c r="J72" s="70"/>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="70"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="70"/>
+      <c r="E73" s="70"/>
+      <c r="F73" s="70"/>
+      <c r="G73" s="70"/>
+      <c r="H73" s="70"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="70"/>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" s="70"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
+      <c r="F74" s="70"/>
+      <c r="G74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="I74" s="70"/>
+      <c r="J74" s="70"/>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="70"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="70"/>
+      <c r="G75" s="70"/>
+      <c r="H75" s="70"/>
+      <c r="I75" s="70"/>
+      <c r="J75" s="70"/>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" s="70"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="70"/>
+      <c r="E76" s="70"/>
+      <c r="F76" s="70"/>
+      <c r="G76" s="70"/>
+      <c r="H76" s="70"/>
+      <c r="I76" s="70"/>
+      <c r="J76" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B45:J76"/>
-    <mergeCell ref="B44:J44"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
+  <mergeCells count="30">
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="E33:J33"/>
     <mergeCell ref="E34:I34"/>
     <mergeCell ref="E35:I35"/>
@@ -5228,24 +5245,23 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="E21:J30"/>
     <mergeCell ref="B31:C35"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B45:J76"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5253,62 +5269,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" ht="18.5">
       <c r="B4" s="28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31">
       <c r="B8" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="18.5" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18.5">
       <c r="B10" s="66" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" s="66"/>
       <c r="D10" s="66"/>
@@ -5316,125 +5332,125 @@
       <c r="F10" s="66"/>
       <c r="G10" s="66"/>
     </row>
-    <row r="11" spans="2:7" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="89"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="91"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="409.5" customHeight="1">
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="90"/>
+    </row>
+    <row r="12" spans="2:7">
       <c r="E12" s="36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" ht="18.5">
       <c r="B13" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="F13" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="31">
       <c r="B14" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31">
       <c r="B15" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="31">
       <c r="B16" s="15" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="31">
       <c r="B17" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" s="15"/>
       <c r="C18" s="11"/>
       <c r="E18" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" s="1"/>
       <c r="E19" s="53" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5444,6 +5460,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5451,35 +5472,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.83203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="29.33203125" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.5">
-      <c r="B3" s="79" t="s">
+    <row r="3" spans="2:9" ht="21">
+      <c r="B3" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-    </row>
-    <row r="4" spans="2:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+    </row>
+    <row r="4" spans="2:9" ht="18.5">
       <c r="B4" s="66" t="s">
         <v>60</v>
       </c>
@@ -5493,81 +5514,81 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="94" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
+    <row r="5" spans="2:9" s="20" customFormat="1">
+      <c r="B5" s="93" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
       <c r="I5" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="94" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
+    <row r="6" spans="2:9" s="20" customFormat="1">
+      <c r="B6" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
       <c r="I6" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="95" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
+    <row r="7" spans="2:9" s="20" customFormat="1">
+      <c r="B7" s="94" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
       <c r="I7" s="30">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="94" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
+    <row r="8" spans="2:9" s="20" customFormat="1">
+      <c r="B8" s="93" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
       <c r="I8" s="30">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="94" t="s">
+    <row r="9" spans="2:9" s="20" customFormat="1">
+      <c r="B9" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
       <c r="I9" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="20" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B10" s="97" t="s">
+    <row r="10" spans="2:9" s="20" customFormat="1" ht="18.5">
+      <c r="B10" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="97"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="66" t="s">
         <v>59</v>
       </c>
@@ -5577,9 +5598,9 @@
       <c r="H10" s="66"/>
       <c r="I10" s="66"/>
     </row>
-    <row r="11" spans="2:9" s="20" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="97"/>
-      <c r="C11" s="97"/>
+    <row r="11" spans="2:9" s="20" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="19" t="s">
         <v>29</v>
       </c>
@@ -5599,60 +5620,60 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="69" t="s">
+    <row r="12" spans="2:9" s="20" customFormat="1">
+      <c r="B12" s="83" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="69"/>
+    <row r="13" spans="2:9" s="20" customFormat="1">
+      <c r="B13" s="83"/>
       <c r="C13" s="11" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="69"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="20" customFormat="1">
+      <c r="B14" s="83"/>
       <c r="C14" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
     </row>
-    <row r="15" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="69"/>
+    <row r="15" spans="2:9" s="20" customFormat="1">
+      <c r="B15" s="83"/>
       <c r="C15" s="11" t="s">
         <v>55</v>
       </c>
@@ -5663,10 +5684,10 @@
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="69"/>
+    <row r="16" spans="2:9" s="20" customFormat="1">
+      <c r="B16" s="83"/>
       <c r="C16" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -5675,8 +5696,8 @@
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="69"/>
+    <row r="17" spans="2:9" s="20" customFormat="1">
+      <c r="B17" s="83"/>
       <c r="C17" s="11" t="s">
         <v>56</v>
       </c>
@@ -5687,23 +5708,23 @@
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>
-    <row r="18" spans="2:9" s="20" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="B18" s="69"/>
+    <row r="18" spans="2:9" s="20" customFormat="1" ht="31">
+      <c r="B18" s="83"/>
       <c r="C18" s="39" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="20" customFormat="1">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="31"/>
@@ -5713,139 +5734,139 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" s="20" customFormat="1">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="2:9" s="20" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" s="20" customFormat="1" ht="18.5">
       <c r="B21" s="28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" s="66" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D21" s="66"/>
       <c r="E21" s="31"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="2:9" s="20" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" s="20" customFormat="1" ht="66" customHeight="1">
       <c r="B22" s="38" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="67" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D22" s="67"/>
       <c r="E22" s="54"/>
       <c r="F22" s="56"/>
       <c r="I22" s="31"/>
     </row>
-    <row r="23" spans="2:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" s="20" customFormat="1">
       <c r="B23" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="96" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="96"/>
+        <v>161</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="95"/>
       <c r="E23" s="31"/>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9" s="20" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" s="20" customFormat="1" ht="31" customHeight="1">
       <c r="B24" s="39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D24" s="67"/>
       <c r="E24" s="31"/>
       <c r="I24" s="31"/>
     </row>
-    <row r="25" spans="2:9" s="20" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" s="20" customFormat="1" ht="31" customHeight="1">
       <c r="B25" s="39" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D25" s="67"/>
       <c r="E25" s="31"/>
       <c r="I25" s="31"/>
     </row>
-    <row r="26" spans="2:9" s="10" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" s="10" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="27" spans="2:9" ht="15.75" customHeight="1">
       <c r="B27" s="62" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" s="63"/>
       <c r="D27" s="64"/>
     </row>
-    <row r="28" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="15.75" customHeight="1">
       <c r="B28" s="33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C28" s="34"/>
       <c r="D28" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="D29" s="55" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="91" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="93"/>
-      <c r="D29" s="55" t="s">
+      <c r="C30" s="92"/>
+      <c r="D30" s="25" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B30" s="92" t="s">
+    <row r="31" spans="2:9">
+      <c r="B31" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="92"/>
+      <c r="D31" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="93"/>
-      <c r="D30" s="25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B31" s="92" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="92" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="92"/>
       <c r="D32" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="C33" s="93"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="92"/>
       <c r="D33" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9">
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
@@ -5854,11 +5875,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B8:H8"/>
@@ -5875,10 +5891,20 @@
     <mergeCell ref="D10:I10"/>
     <mergeCell ref="B12:B18"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5886,22 +5912,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="40.08203125" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="27.9140625" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
     <col min="7" max="7" width="23.5" customWidth="1"/>
-    <col min="8" max="8" width="32.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" ht="18.5">
       <c r="F2" s="66" t="s">
         <v>33</v>
       </c>
@@ -5909,50 +5935,50 @@
       <c r="H2" s="66"/>
       <c r="I2" s="66"/>
     </row>
-    <row r="3" spans="2:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" ht="18.5">
       <c r="B3" s="28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D3" s="52"/>
       <c r="F3" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="99" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="99"/>
-    </row>
-    <row r="4" spans="2:9" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+      <c r="H3" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="98"/>
+    </row>
+    <row r="4" spans="2:9" ht="32" customHeight="1">
       <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" s="67"/>
       <c r="F4" s="23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="H4" s="98" t="s">
-        <v>174</v>
-      </c>
-      <c r="I4" s="98"/>
-    </row>
-    <row r="5" spans="2:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="H4" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="97"/>
+    </row>
+    <row r="5" spans="2:9" ht="32.5" customHeight="1">
       <c r="B5" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D5" s="67"/>
       <c r="F5" s="23"/>
@@ -5971,5 +5997,10 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>